<commit_message>
Using deregressedBLUPs as input "ydBLUPs"
</commit_message>
<xml_diff>
--- a/GS_cor.xlsx
+++ b/GS_cor.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="1780" windowWidth="22400" windowHeight="10600" tabRatio="500"/>
+    <workbookView minimized="1" xWindow="4720" yWindow="520" windowWidth="23420" windowHeight="13580" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Without_FMLoc_cor_BLUE_raw_mode" sheetId="1" r:id="rId1"/>
+    <sheet name="GS_cor_Table" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>All_itself</t>
   </si>
@@ -106,14 +107,45 @@
   </si>
   <si>
     <t>percDw</t>
+  </si>
+  <si>
+    <t>2020 CV</t>
+  </si>
+  <si>
+    <t>2019CV</t>
+  </si>
+  <si>
+    <t>wetWgtPerM</t>
+  </si>
+  <si>
+    <t>percDryWgt</t>
+  </si>
+  <si>
+    <t>AshFDwPM</t>
+  </si>
+  <si>
+    <t>dryWgtPerM</t>
+  </si>
+  <si>
+    <t>Ash</t>
+  </si>
+  <si>
+    <t>BothYerCV</t>
+  </si>
+  <si>
+    <t>BothYearCV</t>
+  </si>
+  <si>
+    <t>March18Collected:</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -178,7 +210,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -186,8 +218,88 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="31">
+  <cellStyleXfs count="47">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -219,8 +331,24 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -236,8 +364,21 @@
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="31">
+  <cellStyles count="47">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -253,6 +394,14 @@
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -268,6 +417,14 @@
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -597,10 +754,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P22"/>
+  <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7:C8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -608,6 +765,7 @@
     <col min="1" max="1" width="29.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="13.5" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
   </cols>
@@ -836,10 +994,10 @@
       <c r="I6" s="9">
         <v>-2.6646980000000001E-2</v>
       </c>
-      <c r="J6" s="11">
+      <c r="J6" s="15">
         <v>0.36812455999999999</v>
       </c>
-      <c r="K6" s="9">
+      <c r="K6" s="15">
         <v>0.36830868</v>
       </c>
       <c r="L6" s="9">
@@ -967,17 +1125,17 @@
         <v>3.6138939999999999E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:5">
+    <row r="18" spans="1:6">
       <c r="A18" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:5">
+    <row r="19" spans="1:6">
       <c r="A19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:5">
+    <row r="20" spans="1:6">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -994,9 +1152,233 @@
         <v>3.16585E-3</v>
       </c>
     </row>
-    <row r="22" spans="1:5">
+    <row r="22" spans="1:6">
       <c r="A22" s="2" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="B27" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="C27" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D27" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="E27" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F27" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" s="20"/>
+      <c r="B28" s="21">
+        <v>0.48663010000000001</v>
+      </c>
+      <c r="C28" s="21">
+        <v>0.26253989999999999</v>
+      </c>
+      <c r="D28" s="21">
+        <v>0.5070192</v>
+      </c>
+      <c r="E28" s="21">
+        <v>0.18109900000000001</v>
+      </c>
+      <c r="F28" s="22">
+        <v>0.40025309999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C29" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D29" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E29" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F29" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="20"/>
+      <c r="B30" s="21">
+        <v>0.21439037999999999</v>
+      </c>
+      <c r="C30" s="21">
+        <v>0.10749791</v>
+      </c>
+      <c r="D30" s="21">
+        <v>0.22539936999999999</v>
+      </c>
+      <c r="E30" s="21">
+        <v>-1.119566E-2</v>
+      </c>
+      <c r="F30" s="22">
+        <v>0.30113239000000003</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" s="20" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" s="23" t="s">
+        <v>34</v>
+      </c>
+      <c r="E31" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F31" s="24" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" s="25"/>
+      <c r="B32" s="26">
+        <v>0.42884562100000001</v>
+      </c>
+      <c r="C32" s="26">
+        <v>7.0054729999999999E-3</v>
+      </c>
+      <c r="D32" s="26">
+        <v>0.44642919399999997</v>
+      </c>
+      <c r="E32" s="26">
+        <v>0.20498957200000001</v>
+      </c>
+      <c r="F32" s="27">
+        <v>0.178031726</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="B1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="16">
+        <v>0.48663010000000001</v>
+      </c>
+      <c r="C2" s="16">
+        <v>0.21439037999999999</v>
+      </c>
+      <c r="D2" s="16">
+        <v>0.42884562100000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="16">
+        <v>0.26253989999999999</v>
+      </c>
+      <c r="C3" s="16">
+        <v>0.10749791</v>
+      </c>
+      <c r="D3" s="16">
+        <v>7.0054729999999999E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>34</v>
+      </c>
+      <c r="B4" s="16">
+        <v>0.5070192</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0.22539936999999999</v>
+      </c>
+      <c r="D4" s="16">
+        <v>0.44642919399999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="16">
+        <v>0.18109900000000001</v>
+      </c>
+      <c r="C5" s="16">
+        <v>-1.119566E-2</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0.20498957200000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="16">
+        <v>0.40025309999999997</v>
+      </c>
+      <c r="C6" s="16">
+        <v>0.30113239000000003</v>
+      </c>
+      <c r="D6" s="16">
+        <v>0.178031726</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Finish dBLUPs and GS runs
</commit_message>
<xml_diff>
--- a/GS_cor.xlsx
+++ b/GS_cor.xlsx
@@ -4,11 +4,14 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="4720" yWindow="520" windowWidth="23420" windowHeight="13580" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="1900" yWindow="800" windowWidth="23420" windowHeight="14560" tabRatio="500" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Without_FMLoc_cor_BLUE_raw_mode" sheetId="1" r:id="rId1"/>
     <sheet name="GS_cor_Table" sheetId="2" r:id="rId2"/>
+    <sheet name="Table1a, 2" sheetId="4" r:id="rId3"/>
+    <sheet name="Table1b" sheetId="5" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="82">
   <si>
     <t>All_itself</t>
   </si>
@@ -137,6 +140,135 @@
   </si>
   <si>
     <t>March18Collected:</t>
+  </si>
+  <si>
+    <t>bladeLength</t>
+  </si>
+  <si>
+    <t>bladeMaxWidth</t>
+  </si>
+  <si>
+    <t>bladeThickness</t>
+  </si>
+  <si>
+    <t>stipeLength</t>
+  </si>
+  <si>
+    <t>stipeDiameter</t>
+  </si>
+  <si>
+    <t>Genetic_Cor_Yr19,Yr20</t>
+  </si>
+  <si>
+    <t>AshOnly</t>
+  </si>
+  <si>
+    <t>wetWgtPlot</t>
+  </si>
+  <si>
+    <t>plotDensity</t>
+  </si>
+  <si>
+    <t>SampleSize</t>
+  </si>
+  <si>
+    <t>Both Yr</t>
+  </si>
+  <si>
+    <t>GS r</t>
+  </si>
+  <si>
+    <t>USE BLUEs</t>
+  </si>
+  <si>
+    <t>TP</t>
+  </si>
+  <si>
+    <t>PP</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t>Yr2019</t>
+  </si>
+  <si>
+    <t>Yr2020</t>
+  </si>
+  <si>
+    <t>Scheme</t>
+  </si>
+  <si>
+    <t>10fold-CV</t>
+  </si>
+  <si>
+    <t>One time</t>
+  </si>
+  <si>
+    <t>Supplemental Table</t>
+  </si>
+  <si>
+    <t>Heritability</t>
+  </si>
+  <si>
+    <t>WWP</t>
+  </si>
+  <si>
+    <t>pDW</t>
+  </si>
+  <si>
+    <t>DWpM</t>
+  </si>
+  <si>
+    <t>AshFDWpM</t>
+  </si>
+  <si>
+    <t>DP</t>
+  </si>
+  <si>
+    <t>BmWid</t>
+  </si>
+  <si>
+    <t>BTh</t>
+  </si>
+  <si>
+    <t>SDia</t>
+  </si>
+  <si>
+    <t>Slen</t>
+  </si>
+  <si>
+    <t>Blen</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>NC</t>
+  </si>
+  <si>
+    <t>NL</t>
+  </si>
+  <si>
+    <t>JS</t>
+  </si>
+  <si>
+    <t>OI</t>
+  </si>
+  <si>
+    <t>SF</t>
+  </si>
+  <si>
+    <t>LD</t>
+  </si>
+  <si>
+    <t>CB</t>
+  </si>
+  <si>
+    <t>Within Year dBLUPs Data</t>
+  </si>
+  <si>
+    <t>Both Years dBLUPs data ---- Trend is the same</t>
   </si>
 </sst>
 </file>
@@ -147,7 +279,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -189,8 +321,31 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Cambria"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -209,8 +364,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="9">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -298,8 +465,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="47">
+  <cellStyleXfs count="209">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -347,8 +566,170 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -377,8 +758,34 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="6" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="5" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="47">
+  <cellStyles count="209">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -402,6 +809,87 @@
     <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -425,6 +913,87 @@
     <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -756,8 +1325,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1289,96 +1858,1445 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:N29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:D4"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:N15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1640625" customWidth="1"/>
+    <col min="4" max="4" width="10" customWidth="1"/>
+    <col min="5" max="5" width="8" customWidth="1"/>
+    <col min="6" max="6" width="8.1640625" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" customWidth="1"/>
+    <col min="8" max="8" width="9" customWidth="1"/>
+    <col min="9" max="9" width="8" customWidth="1"/>
+    <col min="10" max="10" width="6.83203125" customWidth="1"/>
+    <col min="11" max="11" width="8.5" customWidth="1"/>
+    <col min="12" max="12" width="7.5" customWidth="1"/>
+    <col min="13" max="13" width="6" customWidth="1"/>
+    <col min="14" max="14" width="7.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="B1" t="s">
+    <row r="1" spans="1:14">
+      <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" t="s">
         <v>37</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
         <v>29</v>
       </c>
-      <c r="D1" t="s">
+      <c r="F1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:14">
       <c r="A2" t="s">
         <v>31</v>
       </c>
-      <c r="B2" s="16">
+      <c r="D2" s="16">
         <v>0.48663010000000001</v>
       </c>
-      <c r="C2" s="16">
+      <c r="E2" s="16">
         <v>0.21439037999999999</v>
       </c>
-      <c r="D2" s="16">
+      <c r="F2" s="16">
         <v>0.42884562100000001</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:14">
       <c r="A3" t="s">
         <v>32</v>
       </c>
-      <c r="B3" s="16">
+      <c r="D3" s="16">
         <v>0.26253989999999999</v>
       </c>
-      <c r="C3" s="16">
+      <c r="E3" s="16">
         <v>0.10749791</v>
       </c>
-      <c r="D3" s="16">
+      <c r="F3" s="16">
         <v>7.0054729999999999E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:14">
       <c r="A4" t="s">
         <v>34</v>
       </c>
-      <c r="B4" s="16">
+      <c r="D4" s="16">
         <v>0.5070192</v>
       </c>
-      <c r="C4" s="16">
+      <c r="E4" s="16">
         <v>0.22539936999999999</v>
       </c>
-      <c r="D4" s="16">
+      <c r="F4" s="16">
         <v>0.44642919399999997</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:14">
       <c r="A5" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="16">
+      <c r="D5" s="16">
         <v>0.18109900000000001</v>
       </c>
-      <c r="C5" s="16">
+      <c r="E5" s="16">
         <v>-1.119566E-2</v>
       </c>
-      <c r="D5" s="16">
+      <c r="F5" s="16">
         <v>0.20498957200000001</v>
       </c>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:14">
       <c r="A6" t="s">
         <v>33</v>
       </c>
-      <c r="B6" s="16">
+      <c r="D6" s="16">
         <v>0.40025309999999997</v>
       </c>
-      <c r="C6" s="16">
+      <c r="E6" s="16">
         <v>0.30113239000000003</v>
       </c>
-      <c r="D6" s="16">
+      <c r="F6" s="16">
         <v>0.178031726</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14">
+      <c r="A9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14">
+      <c r="A10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+      <c r="G10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H10" t="s">
+        <v>33</v>
+      </c>
+      <c r="J10" t="s">
+        <v>39</v>
+      </c>
+      <c r="K10" t="s">
+        <v>40</v>
+      </c>
+      <c r="L10" t="s">
+        <v>41</v>
+      </c>
+      <c r="M10" t="s">
+        <v>42</v>
+      </c>
+      <c r="N10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14">
+      <c r="A11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" t="s">
+        <v>58</v>
+      </c>
+      <c r="D11" s="16">
+        <v>0.2501467</v>
+      </c>
+      <c r="E11" s="16">
+        <v>0.12640599999999999</v>
+      </c>
+      <c r="F11" s="16">
+        <v>0.23578479999999999</v>
+      </c>
+      <c r="G11" s="16">
+        <v>0.15196879999999999</v>
+      </c>
+      <c r="H11" s="16">
+        <v>0.2325911</v>
+      </c>
+      <c r="I11" s="16"/>
+      <c r="J11" s="16">
+        <v>0.16589719999999999</v>
+      </c>
+      <c r="K11" s="16">
+        <v>0.1450456</v>
+      </c>
+      <c r="L11" s="16">
+        <v>0.34828480000000001</v>
+      </c>
+      <c r="M11" s="16">
+        <v>0.12150469999999999</v>
+      </c>
+      <c r="N11" s="16">
+        <v>0.56684579999999996</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" t="s">
+        <v>55</v>
+      </c>
+      <c r="B12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12" s="16">
+        <v>0.39962706999999997</v>
+      </c>
+      <c r="E12" s="16">
+        <v>-0.14723290999999999</v>
+      </c>
+      <c r="F12" s="16">
+        <v>0.39441457000000002</v>
+      </c>
+      <c r="G12" s="29">
+        <v>0.29764527000000002</v>
+      </c>
+      <c r="H12" s="29">
+        <v>6.5948629999999994E-2</v>
+      </c>
+      <c r="I12" s="16"/>
+      <c r="J12" s="16">
+        <v>0.36490926000000001</v>
+      </c>
+      <c r="K12" s="16">
+        <v>0.29176737000000003</v>
+      </c>
+      <c r="L12" s="16">
+        <v>0.23585089000000001</v>
+      </c>
+      <c r="M12" s="16">
+        <v>2.1358909999999998E-2</v>
+      </c>
+      <c r="N12" s="16">
+        <v>0.37335259999999998</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" t="s">
+        <v>58</v>
+      </c>
+      <c r="D13" s="16">
+        <v>0.19333022999999999</v>
+      </c>
+      <c r="E13" s="16">
+        <v>0.11329314</v>
+      </c>
+      <c r="F13" s="16">
+        <v>0.18848839000000001</v>
+      </c>
+      <c r="G13" s="31">
+        <v>6.4254900000000004E-2</v>
+      </c>
+      <c r="H13" s="31">
+        <v>0.19723303</v>
+      </c>
+      <c r="I13" s="16"/>
+      <c r="J13" s="16">
+        <v>0.12728033999999999</v>
+      </c>
+      <c r="K13" s="16">
+        <v>-1.6349510000000001E-2</v>
+      </c>
+      <c r="L13" s="16">
+        <v>0.38915548</v>
+      </c>
+      <c r="M13" s="16">
+        <v>4.3347379999999998E-2</v>
+      </c>
+      <c r="N13" s="16">
+        <v>0.53816459999999999</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="16">
+        <v>2.4228999000000001E-2</v>
+      </c>
+      <c r="E14" s="16">
+        <v>-5.5982560000000001E-2</v>
+      </c>
+      <c r="F14" s="16">
+        <v>-3.0334008999999999E-2</v>
+      </c>
+      <c r="G14" s="16">
+        <v>8.5934789999999994E-3</v>
+      </c>
+      <c r="H14" s="16">
+        <v>-0.156983975</v>
+      </c>
+      <c r="I14" s="16"/>
+      <c r="J14" s="16">
+        <v>4.9887158000000001E-2</v>
+      </c>
+      <c r="K14" s="16">
+        <v>6.2814691000000006E-2</v>
+      </c>
+      <c r="L14" s="16">
+        <v>-1.9668954999999998E-2</v>
+      </c>
+      <c r="M14" s="16">
+        <v>4.1036568000000002E-2</v>
+      </c>
+      <c r="N14" s="16">
+        <v>0.195411002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" t="s">
+        <v>56</v>
+      </c>
+      <c r="B15" t="s">
+        <v>55</v>
+      </c>
+      <c r="C15" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="16">
+        <v>-2.4928783999999999E-2</v>
+      </c>
+      <c r="E15" s="16">
+        <v>-0.13669815699999999</v>
+      </c>
+      <c r="F15" s="16">
+        <v>-0.11896686200000001</v>
+      </c>
+      <c r="G15" s="16">
+        <v>6.9665464999999996E-2</v>
+      </c>
+      <c r="H15" s="16">
+        <v>-0.25059633100000001</v>
+      </c>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16">
+        <v>1.6414115999999999E-2</v>
+      </c>
+      <c r="K15" s="16">
+        <v>0.152523872</v>
+      </c>
+      <c r="L15" s="16">
+        <v>-9.8783667000000006E-2</v>
+      </c>
+      <c r="M15" s="16">
+        <v>9.2510820000000007E-3</v>
+      </c>
+      <c r="N15" s="16">
+        <v>0.16572218599999999</v>
+      </c>
+    </row>
+    <row r="19" spans="3:14">
+      <c r="C19" t="s">
+        <v>61</v>
+      </c>
+      <c r="D19" t="s">
+        <v>46</v>
+      </c>
+      <c r="E19" t="s">
+        <v>32</v>
+      </c>
+      <c r="F19" t="s">
+        <v>34</v>
+      </c>
+      <c r="G19" t="s">
+        <v>45</v>
+      </c>
+      <c r="H19" t="s">
+        <v>33</v>
+      </c>
+      <c r="I19" t="s">
+        <v>47</v>
+      </c>
+      <c r="J19" t="s">
+        <v>39</v>
+      </c>
+      <c r="K19" t="s">
+        <v>40</v>
+      </c>
+      <c r="L19" t="s">
+        <v>41</v>
+      </c>
+      <c r="M19" t="s">
+        <v>42</v>
+      </c>
+      <c r="N19" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="20" spans="3:14">
+      <c r="C20" t="s">
+        <v>55</v>
+      </c>
+      <c r="D20" s="30">
+        <v>0.50906456899999997</v>
+      </c>
+      <c r="E20" s="30">
+        <v>4.5551248000000003E-2</v>
+      </c>
+      <c r="F20" s="30">
+        <v>0.45186009399999999</v>
+      </c>
+      <c r="G20" s="30">
+        <v>0.201400259</v>
+      </c>
+      <c r="H20" s="30">
+        <v>5.1015240000000003E-2</v>
+      </c>
+      <c r="I20" s="16">
+        <v>0.27622069399999999</v>
+      </c>
+      <c r="J20" s="16">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="K20" s="16">
+        <v>0.106</v>
+      </c>
+      <c r="L20" s="16">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="M20" s="16">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="N20" s="16">
+        <v>0.46400000000000002</v>
+      </c>
+    </row>
+    <row r="21" spans="3:14">
+      <c r="C21" t="s">
+        <v>56</v>
+      </c>
+      <c r="D21" s="16">
+        <v>0.40308374531233399</v>
+      </c>
+      <c r="E21" s="16">
+        <v>0.23846880471901899</v>
+      </c>
+      <c r="F21" s="16">
+        <v>0.35231810262805102</v>
+      </c>
+      <c r="G21" s="16">
+        <v>0.182682176025878</v>
+      </c>
+      <c r="H21" s="16">
+        <v>0.36197062136677399</v>
+      </c>
+      <c r="I21" s="16">
+        <v>0.26920771500000001</v>
+      </c>
+      <c r="J21" s="16">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="K21" s="16">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="L21" s="16">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="M21" s="16">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="N21" s="16">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="22" spans="3:14">
+      <c r="C22" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="16">
+        <v>0.51623591010438896</v>
+      </c>
+      <c r="E22" s="16">
+        <v>5.6691041921284401E-2</v>
+      </c>
+      <c r="F22" s="16">
+        <v>0.45569240959622798</v>
+      </c>
+      <c r="G22" s="16">
+        <v>0.135398162241777</v>
+      </c>
+      <c r="H22" s="16">
+        <v>0.300192260761657</v>
+      </c>
+      <c r="I22" s="16">
+        <v>0.216932554</v>
+      </c>
+      <c r="J22" s="16">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="K22" s="16">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="L22" s="16">
+        <v>0.53</v>
+      </c>
+      <c r="M22" s="16">
+        <v>0.42</v>
+      </c>
+      <c r="N22" s="16">
+        <v>0.65600000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="3:14">
+      <c r="C23" t="s">
+        <v>44</v>
+      </c>
+      <c r="D23" s="16">
+        <v>0.6361194</v>
+      </c>
+      <c r="E23" s="16">
+        <v>-0.7690806</v>
+      </c>
+      <c r="F23" s="16">
+        <v>0.49064219999999997</v>
+      </c>
+      <c r="G23" s="16">
+        <v>-0.52132920000000005</v>
+      </c>
+      <c r="H23" s="16">
+        <v>-0.50211510000000004</v>
+      </c>
+      <c r="I23" s="28">
+        <v>0.24265120000000001</v>
+      </c>
+      <c r="J23" s="16">
+        <v>0.28266340000000001</v>
+      </c>
+      <c r="K23" s="16">
+        <v>0.20119039999999999</v>
+      </c>
+      <c r="L23" s="16">
+        <v>0.27186320000000003</v>
+      </c>
+      <c r="M23" s="16">
+        <v>0.59569830000000001</v>
+      </c>
+      <c r="N23" s="16">
+        <v>0.67725690000000005</v>
+      </c>
+    </row>
+    <row r="25" spans="3:14">
+      <c r="C25" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="3:14">
+      <c r="C26" t="s">
+        <v>48</v>
+      </c>
+      <c r="D26" t="s">
+        <v>46</v>
+      </c>
+      <c r="E26" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" t="s">
+        <v>45</v>
+      </c>
+      <c r="H26" t="s">
+        <v>33</v>
+      </c>
+      <c r="I26" t="s">
+        <v>47</v>
+      </c>
+      <c r="J26" t="s">
+        <v>39</v>
+      </c>
+      <c r="K26" t="s">
+        <v>40</v>
+      </c>
+      <c r="L26" t="s">
+        <v>41</v>
+      </c>
+      <c r="M26" t="s">
+        <v>42</v>
+      </c>
+      <c r="N26" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="27" spans="3:14">
+      <c r="C27" t="s">
+        <v>55</v>
+      </c>
+      <c r="D27">
+        <v>122</v>
+      </c>
+      <c r="E27">
+        <v>122</v>
+      </c>
+      <c r="F27">
+        <v>122</v>
+      </c>
+      <c r="G27">
+        <v>45</v>
+      </c>
+      <c r="H27">
+        <v>45</v>
+      </c>
+      <c r="J27">
+        <v>122</v>
+      </c>
+      <c r="K27">
+        <v>122</v>
+      </c>
+      <c r="L27">
+        <v>122</v>
+      </c>
+      <c r="M27">
+        <v>122</v>
+      </c>
+      <c r="N27">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="28" spans="3:14">
+      <c r="C28" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28">
+        <v>126</v>
+      </c>
+      <c r="E28">
+        <v>126</v>
+      </c>
+      <c r="F28">
+        <v>126</v>
+      </c>
+      <c r="G28">
+        <v>124</v>
+      </c>
+      <c r="H28">
+        <v>123</v>
+      </c>
+      <c r="J28">
+        <v>127</v>
+      </c>
+      <c r="K28">
+        <v>127</v>
+      </c>
+      <c r="L28">
+        <v>127</v>
+      </c>
+      <c r="M28">
+        <v>127</v>
+      </c>
+      <c r="N28">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="29" spans="3:14">
+      <c r="C29" t="s">
+        <v>49</v>
+      </c>
+      <c r="D29">
+        <v>243</v>
+      </c>
+      <c r="E29">
+        <v>243</v>
+      </c>
+      <c r="F29">
+        <v>243</v>
+      </c>
+      <c r="G29">
+        <v>165</v>
+      </c>
+      <c r="H29">
+        <v>164</v>
+      </c>
+      <c r="J29">
+        <v>244</v>
+      </c>
+      <c r="K29">
+        <v>244</v>
+      </c>
+      <c r="L29">
+        <v>244</v>
+      </c>
+      <c r="M29">
+        <v>244</v>
+      </c>
+      <c r="N29">
+        <v>244</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="D11:N13">
+    <cfRule type="colorScale" priority="4">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D23:N23">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D22:N22">
+    <cfRule type="colorScale" priority="5">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="D20:N22">
+    <cfRule type="colorScale" priority="6">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14:N14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14">
+      <c r="A1" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="10" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" s="10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14">
+      <c r="A2" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B2" s="32">
+        <v>0.50906456899999997</v>
+      </c>
+      <c r="C2" s="32">
+        <v>4.5551248000000003E-2</v>
+      </c>
+      <c r="D2" s="32">
+        <v>0.45186009399999999</v>
+      </c>
+      <c r="E2" s="32">
+        <v>0.201400259</v>
+      </c>
+      <c r="F2" s="32">
+        <v>5.1015240000000003E-2</v>
+      </c>
+      <c r="G2" s="33">
+        <v>0.27622069399999999</v>
+      </c>
+      <c r="H2" s="33">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="I2" s="33">
+        <v>0.106</v>
+      </c>
+      <c r="J2" s="33">
+        <v>0.38400000000000001</v>
+      </c>
+      <c r="K2" s="33">
+        <v>0.27400000000000002</v>
+      </c>
+      <c r="L2" s="33">
+        <v>0.46400000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14">
+      <c r="A3" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B3" s="33">
+        <v>0.40308374531233399</v>
+      </c>
+      <c r="C3" s="33">
+        <v>0.23846880471901899</v>
+      </c>
+      <c r="D3" s="33">
+        <v>0.35231810262805102</v>
+      </c>
+      <c r="E3" s="33">
+        <v>0.182682176025878</v>
+      </c>
+      <c r="F3" s="33">
+        <v>0.36197062136677399</v>
+      </c>
+      <c r="G3" s="33">
+        <v>0.26920771500000001</v>
+      </c>
+      <c r="H3" s="33">
+        <v>0.17499999999999999</v>
+      </c>
+      <c r="I3" s="33">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="J3" s="33">
+        <v>0.76600000000000001</v>
+      </c>
+      <c r="K3" s="33">
+        <v>0.55500000000000005</v>
+      </c>
+      <c r="L3" s="33">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14">
+      <c r="A4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="33">
+        <v>0.51623591010438896</v>
+      </c>
+      <c r="C4" s="33">
+        <v>5.6691041921284401E-2</v>
+      </c>
+      <c r="D4" s="33">
+        <v>0.45569240959622798</v>
+      </c>
+      <c r="E4" s="33">
+        <v>0.135398162241777</v>
+      </c>
+      <c r="F4" s="33">
+        <v>0.300192260761657</v>
+      </c>
+      <c r="G4" s="33">
+        <v>0.216932554</v>
+      </c>
+      <c r="H4" s="33">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="I4" s="33">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="J4" s="33">
+        <v>0.53</v>
+      </c>
+      <c r="K4" s="33">
+        <v>0.42</v>
+      </c>
+      <c r="L4" s="33">
+        <v>0.65600000000000003</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14">
+      <c r="A5" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="B5" s="33">
+        <v>0.6361194</v>
+      </c>
+      <c r="C5" s="33">
+        <v>-0.7690806</v>
+      </c>
+      <c r="D5" s="33">
+        <v>0.49064219999999997</v>
+      </c>
+      <c r="E5" s="33">
+        <v>-0.52132920000000005</v>
+      </c>
+      <c r="F5" s="33">
+        <v>-0.50211510000000004</v>
+      </c>
+      <c r="G5" s="33">
+        <v>0.24265120000000001</v>
+      </c>
+      <c r="H5" s="33">
+        <v>0.28266340000000001</v>
+      </c>
+      <c r="I5" s="33">
+        <v>0.20119039999999999</v>
+      </c>
+      <c r="J5" s="33">
+        <v>0.27186320000000003</v>
+      </c>
+      <c r="K5" s="33">
+        <v>0.59569830000000001</v>
+      </c>
+      <c r="L5" s="33">
+        <v>0.67725690000000005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" ht="16" thickBot="1"/>
+    <row r="7" spans="1:14" ht="16" thickBot="1">
+      <c r="A7" s="34" t="s">
+        <v>61</v>
+      </c>
+      <c r="B7" s="35" t="s">
+        <v>62</v>
+      </c>
+      <c r="C7" s="35" t="s">
+        <v>63</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>64</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>65</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>71</v>
+      </c>
+      <c r="I7" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="J7" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="K7" s="35" t="s">
+        <v>70</v>
+      </c>
+      <c r="L7" s="35" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" ht="16" thickBot="1">
+      <c r="A8" s="36" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="37">
+        <v>0.51</v>
+      </c>
+      <c r="C8" s="37">
+        <v>0.05</v>
+      </c>
+      <c r="D8" s="37">
+        <v>0.45</v>
+      </c>
+      <c r="E8" s="37">
+        <v>0.2</v>
+      </c>
+      <c r="F8" s="37">
+        <v>0.05</v>
+      </c>
+      <c r="G8" s="37">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="H8" s="37">
+        <v>0.01</v>
+      </c>
+      <c r="I8" s="37">
+        <v>0.11</v>
+      </c>
+      <c r="J8" s="37">
+        <v>0.38</v>
+      </c>
+      <c r="K8" s="37">
+        <v>0.27</v>
+      </c>
+      <c r="L8" s="37">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" ht="16" thickBot="1">
+      <c r="A9" s="36" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="37">
+        <v>0.4</v>
+      </c>
+      <c r="C9" s="37">
+        <v>0.24</v>
+      </c>
+      <c r="D9" s="37">
+        <v>0.35</v>
+      </c>
+      <c r="E9" s="37">
+        <v>0.18</v>
+      </c>
+      <c r="F9" s="37">
+        <v>0.36</v>
+      </c>
+      <c r="G9" s="37">
+        <v>0.27</v>
+      </c>
+      <c r="H9" s="37">
+        <v>0.18</v>
+      </c>
+      <c r="I9" s="37">
+        <v>0.08</v>
+      </c>
+      <c r="J9" s="37">
+        <v>0.77</v>
+      </c>
+      <c r="K9" s="37">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="L9" s="37">
+        <v>0.82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" ht="16" thickBot="1">
+      <c r="A10" s="36" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="37">
+        <v>0.52</v>
+      </c>
+      <c r="C10" s="37">
+        <v>0.06</v>
+      </c>
+      <c r="D10" s="37">
+        <v>0.46</v>
+      </c>
+      <c r="E10" s="37">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F10" s="37">
+        <v>0.3</v>
+      </c>
+      <c r="G10" s="37">
+        <v>0.22</v>
+      </c>
+      <c r="H10" s="37">
+        <v>0.06</v>
+      </c>
+      <c r="I10" s="37">
+        <v>0.08</v>
+      </c>
+      <c r="J10" s="37">
+        <v>0.53</v>
+      </c>
+      <c r="K10" s="37">
+        <v>0.42</v>
+      </c>
+      <c r="L10" s="37">
+        <v>0.66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" ht="16" thickBot="1">
+      <c r="A11" s="36" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="37">
+        <v>0.64</v>
+      </c>
+      <c r="C11" s="37">
+        <v>-0.77</v>
+      </c>
+      <c r="D11" s="37">
+        <v>0.49</v>
+      </c>
+      <c r="E11" s="37">
+        <v>-0.52</v>
+      </c>
+      <c r="F11" s="37">
+        <v>-0.5</v>
+      </c>
+      <c r="G11" s="37">
+        <v>0.24</v>
+      </c>
+      <c r="H11" s="37">
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="I11" s="37">
+        <v>0.2</v>
+      </c>
+      <c r="J11" s="37">
+        <v>0.27</v>
+      </c>
+      <c r="K11" s="37">
+        <v>0.6</v>
+      </c>
+      <c r="L11" s="37">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14">
+      <c r="A12" s="38"/>
+    </row>
+    <row r="13" spans="1:14" ht="16" thickBot="1">
+      <c r="D13" t="s">
+        <v>31</v>
+      </c>
+      <c r="E13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" t="s">
+        <v>35</v>
+      </c>
+      <c r="H13" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" t="s">
+        <v>39</v>
+      </c>
+      <c r="K13" t="s">
+        <v>40</v>
+      </c>
+      <c r="L13" t="s">
+        <v>41</v>
+      </c>
+      <c r="M13" t="s">
+        <v>42</v>
+      </c>
+      <c r="N13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="16" thickBot="1">
+      <c r="A14" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="B14" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C14" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="D14" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="G14" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="I14" s="39" t="s">
+        <v>66</v>
+      </c>
+      <c r="J14" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="K14" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="L14" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="M14" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="N14" s="39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14">
+      <c r="A15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D15" s="33">
+        <v>0.2501467</v>
+      </c>
+      <c r="E15" s="33">
+        <v>0.12640599999999999</v>
+      </c>
+      <c r="F15" s="33">
+        <v>0.23578479999999999</v>
+      </c>
+      <c r="G15" s="33">
+        <v>0.15196879999999999</v>
+      </c>
+      <c r="H15" s="33">
+        <v>0.2325911</v>
+      </c>
+      <c r="I15" s="33"/>
+      <c r="J15" s="33">
+        <v>0.16589719999999999</v>
+      </c>
+      <c r="K15" s="33">
+        <v>0.1450456</v>
+      </c>
+      <c r="L15" s="33">
+        <v>0.34828480000000001</v>
+      </c>
+      <c r="M15" s="33">
+        <v>0.12150469999999999</v>
+      </c>
+      <c r="N15" s="33">
+        <v>0.56684579999999996</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14">
+      <c r="A16" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D16" s="33">
+        <v>0.39962706999999997</v>
+      </c>
+      <c r="E16" s="33">
+        <v>-0.14723290999999999</v>
+      </c>
+      <c r="F16" s="33">
+        <v>0.39441457000000002</v>
+      </c>
+      <c r="G16" s="40"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="33"/>
+      <c r="J16" s="33">
+        <v>0.36490926000000001</v>
+      </c>
+      <c r="K16" s="33">
+        <v>0.29176737000000003</v>
+      </c>
+      <c r="L16" s="33">
+        <v>0.23585089000000001</v>
+      </c>
+      <c r="M16" s="33">
+        <v>2.1358909999999998E-2</v>
+      </c>
+      <c r="N16" s="33">
+        <v>0.37335259999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14">
+      <c r="A17" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="D17" s="33">
+        <v>0.19333022999999999</v>
+      </c>
+      <c r="E17" s="33">
+        <v>0.11329314</v>
+      </c>
+      <c r="F17" s="33">
+        <v>0.18848839000000001</v>
+      </c>
+      <c r="G17" s="41">
+        <v>6.4254900000000004E-2</v>
+      </c>
+      <c r="H17" s="41">
+        <v>0.19723303</v>
+      </c>
+      <c r="I17" s="33"/>
+      <c r="J17" s="33">
+        <v>0.12728033999999999</v>
+      </c>
+      <c r="K17" s="33">
+        <v>-1.6349510000000001E-2</v>
+      </c>
+      <c r="L17" s="33">
+        <v>0.38915548</v>
+      </c>
+      <c r="M17" s="33">
+        <v>4.3347379999999998E-2</v>
+      </c>
+      <c r="N17" s="33">
+        <v>0.53816459999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14">
+      <c r="A18" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D18" s="33">
+        <v>2.4228999000000001E-2</v>
+      </c>
+      <c r="E18" s="33">
+        <v>-5.5982560000000001E-2</v>
+      </c>
+      <c r="F18" s="33">
+        <v>-3.0334008999999999E-2</v>
+      </c>
+      <c r="G18" s="33">
+        <v>8.5934789999999994E-3</v>
+      </c>
+      <c r="H18" s="33">
+        <v>-0.156983975</v>
+      </c>
+      <c r="I18" s="33"/>
+      <c r="J18" s="33">
+        <v>4.9887158000000001E-2</v>
+      </c>
+      <c r="K18" s="33">
+        <v>6.2814691000000006E-2</v>
+      </c>
+      <c r="L18" s="33">
+        <v>-1.9668954999999998E-2</v>
+      </c>
+      <c r="M18" s="33">
+        <v>4.1036568000000002E-2</v>
+      </c>
+      <c r="N18" s="33">
+        <v>0.195411002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14">
+      <c r="A19" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B19" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D19" s="33">
+        <v>-2.4928783999999999E-2</v>
+      </c>
+      <c r="E19" s="33">
+        <v>-0.13669815699999999</v>
+      </c>
+      <c r="F19" s="33">
+        <v>-0.11896686200000001</v>
+      </c>
+      <c r="G19" s="33">
+        <v>6.9665464999999996E-2</v>
+      </c>
+      <c r="H19" s="33">
+        <v>-0.25059633100000001</v>
+      </c>
+      <c r="I19" s="33"/>
+      <c r="J19" s="33">
+        <v>1.6414115999999999E-2</v>
+      </c>
+      <c r="K19" s="33">
+        <v>0.152523872</v>
+      </c>
+      <c r="L19" s="33">
+        <v>-9.8783667000000006E-2</v>
+      </c>
+      <c r="M19" s="33">
+        <v>9.2510820000000007E-3</v>
+      </c>
+      <c r="N19" s="33">
+        <v>0.16572218599999999</v>
       </c>
     </row>
   </sheetData>
@@ -1390,4 +3308,854 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="C1" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="C2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D2" t="s">
+        <v>68</v>
+      </c>
+      <c r="E2" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" s="16">
+        <v>-0.45370171008414278</v>
+      </c>
+      <c r="D3" s="16">
+        <v>-0.74931107903484295</v>
+      </c>
+      <c r="E3" s="16">
+        <v>-0.24875606907819311</v>
+      </c>
+      <c r="F3" s="16">
+        <v>-0.5357860038838943</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16">
+        <v>-3.0825365952665645E-2</v>
+      </c>
+      <c r="E4" s="16">
+        <v>0.18731283572535865</v>
+      </c>
+      <c r="F4" s="16">
+        <v>-0.40041217423213143</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="16">
+        <v>0.34876621543917913</v>
+      </c>
+      <c r="F5" s="16">
+        <v>0.71557319854545864</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" t="s">
+        <v>42</v>
+      </c>
+      <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" s="16"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="16"/>
+      <c r="F6" s="16">
+        <v>6.0877342241481266E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="3.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="16" thickBot="1">
+      <c r="A1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" t="s">
+        <v>34</v>
+      </c>
+      <c r="E1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+      <c r="L1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="16" thickBot="1">
+      <c r="B2" s="39" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="39" t="s">
+        <v>63</v>
+      </c>
+      <c r="D2" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="E2" s="39" t="s">
+        <v>35</v>
+      </c>
+      <c r="F2" s="39" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39" t="s">
+        <v>71</v>
+      </c>
+      <c r="I2" s="39" t="s">
+        <v>67</v>
+      </c>
+      <c r="J2" s="39" t="s">
+        <v>68</v>
+      </c>
+      <c r="K2" s="39" t="s">
+        <v>70</v>
+      </c>
+      <c r="L2" s="39" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12">
+      <c r="A3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B3" s="16">
+        <v>-4.4729875071212299E-3</v>
+      </c>
+      <c r="C3" s="16">
+        <v>-0.13093257848640499</v>
+      </c>
+      <c r="D3" s="16">
+        <v>-7.7772522539990993E-2</v>
+      </c>
+      <c r="E3" s="16">
+        <v>-9.3559284045157294E-3</v>
+      </c>
+      <c r="F3" s="16">
+        <v>-2.8263186754650001E-2</v>
+      </c>
+      <c r="G3" s="16"/>
+      <c r="H3" s="16">
+        <v>-0.27941280943830499</v>
+      </c>
+      <c r="I3" s="16">
+        <v>0.141955257890754</v>
+      </c>
+      <c r="J3" s="16">
+        <v>0.14440537488564101</v>
+      </c>
+      <c r="K3" s="16">
+        <v>0.234093149119219</v>
+      </c>
+      <c r="L3" s="16">
+        <v>7.6644807507163501E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12">
+      <c r="A4" t="s">
+        <v>73</v>
+      </c>
+      <c r="B4" s="16">
+        <v>0.43506029264061202</v>
+      </c>
+      <c r="C4" s="16">
+        <v>0.33266745112066598</v>
+      </c>
+      <c r="D4" s="16">
+        <v>0.19842534250906499</v>
+      </c>
+      <c r="E4" s="16">
+        <v>-4.4523670213368803E-2</v>
+      </c>
+      <c r="F4" s="16">
+        <v>0.32545757589911101</v>
+      </c>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16">
+        <v>0.155634475822478</v>
+      </c>
+      <c r="I4" s="16">
+        <v>8.2048929603002006E-3</v>
+      </c>
+      <c r="J4" s="16">
+        <v>-4.9047863446479302E-2</v>
+      </c>
+      <c r="K4" s="16">
+        <v>-0.156273158960615</v>
+      </c>
+      <c r="L4" s="16">
+        <v>-3.0493498459023402E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12">
+      <c r="A5" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="16">
+        <v>0.17805534892538499</v>
+      </c>
+      <c r="C5" s="16">
+        <v>0.118173182837941</v>
+      </c>
+      <c r="D5" s="16">
+        <v>0.124245932992209</v>
+      </c>
+      <c r="E5" s="16">
+        <v>2.2141987824081801E-2</v>
+      </c>
+      <c r="F5" s="16">
+        <v>-6.22086103721557E-2</v>
+      </c>
+      <c r="G5" s="16"/>
+      <c r="H5" s="16">
+        <v>-0.104957398903698</v>
+      </c>
+      <c r="I5" s="16">
+        <v>7.4804075359599403E-2</v>
+      </c>
+      <c r="J5" s="16">
+        <v>0.24615259427056599</v>
+      </c>
+      <c r="K5" s="16">
+        <v>0.16929039222757</v>
+      </c>
+      <c r="L5" s="16">
+        <v>0.38091668538928602</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" s="16">
+        <v>-0.17890246342899599</v>
+      </c>
+      <c r="C6" s="16">
+        <v>0.32690907908122002</v>
+      </c>
+      <c r="D6" s="16">
+        <v>2.2848217263813898E-2</v>
+      </c>
+      <c r="E6" s="16">
+        <v>0.13369735569982399</v>
+      </c>
+      <c r="F6" s="16">
+        <v>0.13316601335433101</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16">
+        <v>0.27260531237421098</v>
+      </c>
+      <c r="I6" s="16">
+        <v>0.23789543516056899</v>
+      </c>
+      <c r="J6" s="16">
+        <v>4.68944894931951E-2</v>
+      </c>
+      <c r="K6" s="16">
+        <v>0.24125757376547899</v>
+      </c>
+      <c r="L6" s="16">
+        <v>-0.28996192719202002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12">
+      <c r="A7" t="s">
+        <v>76</v>
+      </c>
+      <c r="B7" s="16">
+        <v>2.9847095249071299E-2</v>
+      </c>
+      <c r="C7" s="16">
+        <v>-0.113121861150541</v>
+      </c>
+      <c r="D7" s="16">
+        <v>-6.0561845075230297E-2</v>
+      </c>
+      <c r="E7" s="16">
+        <v>0.17970573572026899</v>
+      </c>
+      <c r="F7" s="16">
+        <v>-0.20243792257963</v>
+      </c>
+      <c r="G7" s="16"/>
+      <c r="H7" s="16">
+        <v>0.24320044171309199</v>
+      </c>
+      <c r="I7" s="16">
+        <v>9.3430569868122093E-2</v>
+      </c>
+      <c r="J7" s="16">
+        <v>0.131391990686168</v>
+      </c>
+      <c r="K7" s="16">
+        <v>6.1826152884099601E-2</v>
+      </c>
+      <c r="L7" s="16">
+        <v>-6.9094979520718094E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12">
+      <c r="A8" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="16">
+        <v>-5.30455362250254E-3</v>
+      </c>
+      <c r="C8" s="16">
+        <v>4.4422538066077301E-2</v>
+      </c>
+      <c r="D8" s="16">
+        <v>-5.4731496587852001E-2</v>
+      </c>
+      <c r="E8" s="16">
+        <v>-0.29102998263025598</v>
+      </c>
+      <c r="F8" s="16">
+        <v>-5.4643309941758103E-2</v>
+      </c>
+      <c r="G8" s="16"/>
+      <c r="H8" s="16">
+        <v>0.45141915692483198</v>
+      </c>
+      <c r="I8" s="16">
+        <v>-0.32989402213933</v>
+      </c>
+      <c r="J8" s="16">
+        <v>-5.8438123498745699E-2</v>
+      </c>
+      <c r="K8" s="16">
+        <v>0.104061128041367</v>
+      </c>
+      <c r="L8" s="16">
+        <v>-0.61778764728774205</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12">
+      <c r="A9" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="16">
+        <v>0.41489535512132197</v>
+      </c>
+      <c r="C9" s="16">
+        <v>-0.10119589901477601</v>
+      </c>
+      <c r="D9" s="16">
+        <v>0.29658847485607198</v>
+      </c>
+      <c r="E9" s="16">
+        <v>1.6240695365301198E-2</v>
+      </c>
+      <c r="F9" s="16">
+        <v>0.124038842407368</v>
+      </c>
+      <c r="G9" s="16"/>
+      <c r="H9" s="16">
+        <v>0.45615443845961001</v>
+      </c>
+      <c r="I9" s="16">
+        <v>-2.79329253358176E-2</v>
+      </c>
+      <c r="J9" s="16">
+        <v>0.28743830008941301</v>
+      </c>
+      <c r="K9" s="16">
+        <v>-0.13316481440134501</v>
+      </c>
+      <c r="L9" s="16">
+        <v>0.14013313541466599</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>79</v>
+      </c>
+      <c r="B10" s="16">
+        <v>2.9847897899870999E-2</v>
+      </c>
+      <c r="C10" s="16">
+        <v>-3.3824335290755098E-2</v>
+      </c>
+      <c r="D10" s="16">
+        <v>-0.118142362101574</v>
+      </c>
+      <c r="E10" s="16">
+        <v>-5.1329712764978101E-2</v>
+      </c>
+      <c r="F10" s="16">
+        <v>-0.226201856453562</v>
+      </c>
+      <c r="G10" s="16"/>
+      <c r="H10" s="16">
+        <v>-5.4878934060585E-2</v>
+      </c>
+      <c r="I10" s="16">
+        <v>0.31577815623724997</v>
+      </c>
+      <c r="J10" s="16">
+        <v>0.36206960418218997</v>
+      </c>
+      <c r="K10" s="16">
+        <v>0.18614038495562801</v>
+      </c>
+      <c r="L10" s="16">
+        <v>-0.27542237113386098</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
+      <c r="A12" s="2" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
+      <c r="B13" t="s">
+        <v>31</v>
+      </c>
+      <c r="C13" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13" t="s">
+        <v>39</v>
+      </c>
+      <c r="I13" t="s">
+        <v>40</v>
+      </c>
+      <c r="J13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K13" t="s">
+        <v>42</v>
+      </c>
+      <c r="L13" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>72</v>
+      </c>
+      <c r="B14" s="16">
+        <v>-2.87739288441511E-2</v>
+      </c>
+      <c r="C14" s="16">
+        <v>-8.76996449831033E-2</v>
+      </c>
+      <c r="D14" s="16">
+        <v>-3.8265309393836898E-2</v>
+      </c>
+      <c r="E14" s="16">
+        <v>9.6845360790199397E-2</v>
+      </c>
+      <c r="F14" s="16">
+        <v>-5.37764457666495E-2</v>
+      </c>
+      <c r="G14" s="16"/>
+      <c r="H14" s="16">
+        <v>-0.31711823559124502</v>
+      </c>
+      <c r="I14" s="16">
+        <v>0.13343815180965199</v>
+      </c>
+      <c r="J14" s="16">
+        <v>0.197524526195647</v>
+      </c>
+      <c r="K14" s="16">
+        <v>0.26940702630862901</v>
+      </c>
+      <c r="L14" s="16">
+        <v>0.176242686241393</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
+      <c r="A15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B15" s="16">
+        <v>0.200761437234031</v>
+      </c>
+      <c r="C15" s="16">
+        <v>0.51667783061295702</v>
+      </c>
+      <c r="D15" s="16">
+        <v>0.14358687945856399</v>
+      </c>
+      <c r="E15" s="16">
+        <v>6.3927109159953505E-2</v>
+      </c>
+      <c r="F15" s="16">
+        <v>0.23483124457448401</v>
+      </c>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16">
+        <v>0.116837632208597</v>
+      </c>
+      <c r="I15" s="16">
+        <v>0.10708266978987099</v>
+      </c>
+      <c r="J15" s="16">
+        <v>3.8707193539876797E-2</v>
+      </c>
+      <c r="K15" s="16">
+        <v>-0.17246845444990899</v>
+      </c>
+      <c r="L15" s="16">
+        <v>0.308020041999642</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
+      <c r="A16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B16" s="16">
+        <v>0.17904007498153901</v>
+      </c>
+      <c r="C16" s="16">
+        <v>0.17567461904947199</v>
+      </c>
+      <c r="D16" s="16">
+        <v>5.4148500172114401E-2</v>
+      </c>
+      <c r="E16" s="16">
+        <v>-6.05176621081691E-3</v>
+      </c>
+      <c r="F16" s="16">
+        <v>-0.18114863211066101</v>
+      </c>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16">
+        <v>-0.109387505153469</v>
+      </c>
+      <c r="I16" s="16">
+        <v>0.17395500527593499</v>
+      </c>
+      <c r="J16" s="16">
+        <v>0.40752223683744798</v>
+      </c>
+      <c r="K16" s="16">
+        <v>0.16814703816995899</v>
+      </c>
+      <c r="L16" s="16">
+        <v>0.439001362972818</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
+      <c r="A17" t="s">
+        <v>75</v>
+      </c>
+      <c r="B17" s="16">
+        <v>-0.25736545156856599</v>
+      </c>
+      <c r="C17" s="16">
+        <v>0.28883707446829998</v>
+      </c>
+      <c r="D17" s="16">
+        <v>-4.37434635965201E-2</v>
+      </c>
+      <c r="E17" s="16">
+        <v>7.12885593203475E-2</v>
+      </c>
+      <c r="F17" s="16">
+        <v>6.6789290138704896E-2</v>
+      </c>
+      <c r="G17" s="16"/>
+      <c r="H17" s="16">
+        <v>0.245058192623269</v>
+      </c>
+      <c r="I17" s="16">
+        <v>0.21504344133219999</v>
+      </c>
+      <c r="J17" s="16">
+        <v>0.20113211159146399</v>
+      </c>
+      <c r="K17" s="16">
+        <v>0.21209965831095001</v>
+      </c>
+      <c r="L17" s="16">
+        <v>-4.9361903669473899E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12">
+      <c r="A18" t="s">
+        <v>76</v>
+      </c>
+      <c r="B18" s="16">
+        <v>7.8098922363806902E-2</v>
+      </c>
+      <c r="C18" s="16">
+        <v>-0.121873896223142</v>
+      </c>
+      <c r="D18" s="16">
+        <v>1.2109663294425E-2</v>
+      </c>
+      <c r="E18" s="16">
+        <v>0.32574114033186802</v>
+      </c>
+      <c r="F18" s="16">
+        <v>-0.14974965550453601</v>
+      </c>
+      <c r="G18" s="16"/>
+      <c r="H18" s="16">
+        <v>0.27783836036619702</v>
+      </c>
+      <c r="I18" s="16">
+        <v>8.11787578340427E-2</v>
+      </c>
+      <c r="J18" s="16">
+        <v>0.18161593965259901</v>
+      </c>
+      <c r="K18" s="16">
+        <v>0.110833149555656</v>
+      </c>
+      <c r="L18" s="16">
+        <v>-3.6767848346571499E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
+      <c r="A19" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="16">
+        <v>2.79739312087647E-2</v>
+      </c>
+      <c r="C19" s="16">
+        <v>-0.22507761534132301</v>
+      </c>
+      <c r="D19" s="16">
+        <v>-6.1883793432235698E-2</v>
+      </c>
+      <c r="E19" s="16">
+        <v>-0.146105218866563</v>
+      </c>
+      <c r="F19" s="16">
+        <v>-0.131815753309759</v>
+      </c>
+      <c r="G19" s="16"/>
+      <c r="H19" s="16">
+        <v>0.45919503890817698</v>
+      </c>
+      <c r="I19" s="16">
+        <v>-0.27720808756293602</v>
+      </c>
+      <c r="J19" s="16">
+        <v>0.124364620849576</v>
+      </c>
+      <c r="K19" s="16">
+        <v>8.0680672614510798E-2</v>
+      </c>
+      <c r="L19" s="16">
+        <v>-0.55153020203018299</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12">
+      <c r="A20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="16">
+        <v>0.427715885398046</v>
+      </c>
+      <c r="C20" s="16">
+        <v>-0.13407796547766199</v>
+      </c>
+      <c r="D20" s="16">
+        <v>0.44706076109009202</v>
+      </c>
+      <c r="E20" s="16">
+        <v>9.8965118682386402E-2</v>
+      </c>
+      <c r="F20" s="16">
+        <v>0.198382241336239</v>
+      </c>
+      <c r="G20" s="16"/>
+      <c r="H20" s="16">
+        <v>0.49641267848315501</v>
+      </c>
+      <c r="I20" s="16">
+        <v>2.0854400335151398E-2</v>
+      </c>
+      <c r="J20" s="16">
+        <v>0.216018169192396</v>
+      </c>
+      <c r="K20" s="16">
+        <v>-0.102942852820984</v>
+      </c>
+      <c r="L20" s="16">
+        <v>0.214406974933808</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12">
+      <c r="A21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B21" s="16">
+        <v>-5.6331966520346298E-2</v>
+      </c>
+      <c r="C21" s="16">
+        <v>2.68851276575254E-2</v>
+      </c>
+      <c r="D21" s="16">
+        <v>-7.0600169588905401E-2</v>
+      </c>
+      <c r="E21" s="16">
+        <v>7.6717010333781904E-3</v>
+      </c>
+      <c r="F21" s="16">
+        <v>-0.16414177814022099</v>
+      </c>
+      <c r="G21" s="16"/>
+      <c r="H21" s="16">
+        <v>-8.9995790936601705E-2</v>
+      </c>
+      <c r="I21" s="16">
+        <v>0.30887521662420903</v>
+      </c>
+      <c r="J21" s="16">
+        <v>0.54968990812424201</v>
+      </c>
+      <c r="K21" s="16">
+        <v>0.27259007003122698</v>
+      </c>
+      <c r="L21" s="16">
+        <v>-0.178276010418357</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="C14:L21">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B14:L21">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>